<commit_message>
Adding features to classifier models.
</commit_message>
<xml_diff>
--- a/data/classifier_train/broad_assets_ewma_train.xlsx
+++ b/data/classifier_train/broad_assets_ewma_train.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L882"/>
+  <dimension ref="A1:L881"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33941,44 +33941,6 @@
         <v>0.07458789333577893</v>
       </c>
     </row>
-    <row r="882">
-      <c r="A882" s="2" t="n">
-        <v>44004</v>
-      </c>
-      <c r="B882" t="n">
-        <v>0.100959652088968</v>
-      </c>
-      <c r="C882" t="n">
-        <v>0.09332214313915671</v>
-      </c>
-      <c r="D882" t="n">
-        <v>0.0613473612480088</v>
-      </c>
-      <c r="E882" t="n">
-        <v>0.01429630871018052</v>
-      </c>
-      <c r="F882" t="n">
-        <v>0.1483195371644304</v>
-      </c>
-      <c r="G882" t="n">
-        <v>0.1398177735626171</v>
-      </c>
-      <c r="H882" t="n">
-        <v>0.1074917967302695</v>
-      </c>
-      <c r="I882" t="n">
-        <v>0.1041145681034563</v>
-      </c>
-      <c r="J882" t="n">
-        <v>0.02426493479429922</v>
-      </c>
-      <c r="K882" t="n">
-        <v>0.04853915065245717</v>
-      </c>
-      <c r="L882" t="n">
-        <v>0.06696433484760975</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>